<commit_message>
Amélioration export Nouveautés: distinction vrais changements vs recalculs internes
- Nouveaux objets: Type = 'Nouvel objet'
- Changements de statut: Type = 'Statut modifié'
- Autres MAJ: Type = 'Mise à jour contenu'
- Recalculs internes (Mention/Auteur) ignorés
- Ajout colonne Statut dans l'export
</commit_message>
<xml_diff>
--- a/Nouveautés/Nouveautes_2026-02-07.xlsx
+++ b/Nouveautés/Nouveautes_2026-02-07.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
-  <si>
-    <t xml:space="preserve">Type_MAJ</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+  <si>
+    <t xml:space="preserve">Type_Changement</t>
   </si>
   <si>
     <t xml:space="preserve">Numéro</t>
@@ -26,10 +26,13 @@
     <t xml:space="preserve">Mention</t>
   </si>
   <si>
+    <t xml:space="preserve">Statut</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lien_FR</t>
   </si>
   <si>
-    <t xml:space="preserve">Mise à jour</t>
+    <t xml:space="preserve">Mise à jour contenu</t>
   </si>
   <si>
     <t xml:space="preserve">25.3941</t>
@@ -41,6 +44,9 @@
     <t xml:space="preserve">Conseil fédéral</t>
   </si>
   <si>
+    <t xml:space="preserve">Überwiesen an den Bundesrat / Transmis au Conseil fédéral</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20253941</t>
   </si>
   <si>
@@ -53,6 +59,9 @@
     <t xml:space="preserve">Élu &amp; Conseil fédéral</t>
   </si>
   <si>
+    <t xml:space="preserve">Erledigt / Liquidé</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20253971</t>
   </si>
   <si>
@@ -62,6 +71,9 @@
     <t xml:space="preserve">FDP-Liberale Fraktion</t>
   </si>
   <si>
+    <t xml:space="preserve">In Kommission des Ständerats / En commission du Conseil des Etats</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20253984</t>
   </si>
   <si>
@@ -71,6 +83,9 @@
     <t xml:space="preserve">Grünliberale Fraktion</t>
   </si>
   <si>
+    <t xml:space="preserve">Stellungnahme zum Vorstoss liegt vor / L’avis relatif à l’intervention est disponible</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254003</t>
   </si>
   <si>
@@ -107,6 +122,9 @@
     <t xml:space="preserve">Schmid Martin</t>
   </si>
   <si>
+    <t xml:space="preserve">Zugewiesen an die behandelnde Kommission / Attribué à la commission compétente</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254188</t>
   </si>
   <si>
@@ -153,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wettstein Felix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eingereicht / Déposé</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254463</t>
@@ -296,14 +317,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E25" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E25"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Type_MAJ"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F25" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:F25"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Type_Changement"/>
     <tableColumn id="2" name="Numéro"/>
     <tableColumn id="3" name="Auteur"/>
     <tableColumn id="4" name="Mention"/>
-    <tableColumn id="5" name="Lien_FR"/>
+    <tableColumn id="5" name="Statut"/>
+    <tableColumn id="6" name="Lien_FR"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -610,413 +632,488 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
         <v>53</v>
       </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>69</v>
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>